<commit_message>
improve ME analyser.(advanced courses may need to be added in database). Advancec courses shows up in Others.
</commit_message>
<xml_diff>
--- a/database/ME_Course_database.xlsx
+++ b/database/ME_Course_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEE2294-6B6A-44C0-B4AF-1444F88FED85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55898A7F-BF8A-442F-8784-6A11804DBB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t>普通物理學(一)</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>數位邏輯</t>
-  </si>
-  <si>
-    <t>再生能源進階實作專題</t>
   </si>
   <si>
     <t>嵌入式程式設計</t>
@@ -147,9 +144,6 @@
     <t>所有科目</t>
   </si>
   <si>
-    <t>流體力學</t>
-  </si>
-  <si>
     <t>靜力學</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t>普通化學</t>
   </si>
   <si>
-    <t>材料力學</t>
-  </si>
-  <si>
     <t>機械製造</t>
   </si>
   <si>
@@ -196,9 +187,6 @@
   </si>
   <si>
     <t>機械繪圖</t>
-  </si>
-  <si>
-    <t>材料科學</t>
   </si>
   <si>
     <t>機械振動</t>
@@ -253,6 +241,63 @@
   </si>
   <si>
     <t>熱力學二</t>
+  </si>
+  <si>
+    <t>材料科學一</t>
+  </si>
+  <si>
+    <t>材料科學二</t>
+  </si>
+  <si>
+    <t>材料力學二</t>
+  </si>
+  <si>
+    <t>材料力學一</t>
+  </si>
+  <si>
+    <t>機構學</t>
+  </si>
+  <si>
+    <t>自動化科技</t>
+  </si>
+  <si>
+    <t>醫學工程材料</t>
+  </si>
+  <si>
+    <t>流體力學一</t>
+  </si>
+  <si>
+    <t>流體力學二</t>
+  </si>
+  <si>
+    <t>航太工程概論</t>
+  </si>
+  <si>
+    <t>微機電系統理論</t>
+  </si>
+  <si>
+    <t>風力發電</t>
+  </si>
+  <si>
+    <t>電力電子學</t>
+  </si>
+  <si>
+    <t>熱處理技術</t>
+  </si>
+  <si>
+    <t>再生能源系統</t>
+  </si>
+  <si>
+    <t>機械過程預處理</t>
+  </si>
+  <si>
+    <t>材料結構與物性</t>
+  </si>
+  <si>
+    <t>材料性質</t>
+  </si>
+  <si>
+    <t>動態系統分析</t>
   </si>
 </sst>
 </file>
@@ -685,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C323114-BC5F-49C1-9F53-9EA9AB7CC060}">
-  <dimension ref="A1:W415"/>
+  <dimension ref="A1:W424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -699,7 +744,7 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -749,7 +794,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -774,7 +819,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -799,7 +844,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -824,7 +869,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -849,7 +894,7 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="5"/>
       <c r="D7" s="5"/>
@@ -873,7 +918,7 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5"/>
       <c r="D8" s="5"/>
@@ -897,7 +942,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5"/>
       <c r="D9" s="5"/>
@@ -945,7 +990,7 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
@@ -993,7 +1038,7 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="5"/>
       <c r="D13" s="5"/>
@@ -1017,7 +1062,7 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="5"/>
       <c r="D14" s="5"/>
@@ -1041,7 +1086,7 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="5"/>
       <c r="D15" s="5"/>
@@ -1065,7 +1110,7 @@
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B16" s="5"/>
       <c r="D16" s="5"/>
@@ -1089,7 +1134,7 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B17" s="5"/>
       <c r="D17" s="5"/>
@@ -1113,7 +1158,7 @@
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B18" s="5"/>
       <c r="D18" s="5"/>
@@ -1137,7 +1182,7 @@
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="5"/>
       <c r="D19" s="5"/>
@@ -1161,7 +1206,7 @@
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" s="5"/>
       <c r="D20" s="5"/>
@@ -1185,7 +1230,7 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="5"/>
       <c r="D21" s="5"/>
@@ -1209,7 +1254,7 @@
     </row>
     <row r="22" spans="1:23">
       <c r="A22" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="5"/>
       <c r="D22" s="5"/>
@@ -1233,7 +1278,7 @@
     </row>
     <row r="23" spans="1:23">
       <c r="A23" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="5"/>
       <c r="D23" s="5"/>
@@ -1257,7 +1302,7 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" s="9" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="B24" s="5"/>
       <c r="D24" s="5"/>
@@ -1280,8 +1325,8 @@
       <c r="W24" s="7"/>
     </row>
     <row r="25" spans="1:23">
-      <c r="A25" s="10" t="s">
-        <v>26</v>
+      <c r="A25" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="B25" s="5"/>
       <c r="D25" s="5"/>
@@ -1304,8 +1349,8 @@
       <c r="W25" s="7"/>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="9" t="s">
-        <v>33</v>
+      <c r="A26" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="B26" s="5"/>
       <c r="D26" s="5"/>
@@ -1329,7 +1374,7 @@
     </row>
     <row r="27" spans="1:23">
       <c r="A27" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B27" s="5"/>
       <c r="D27" s="5"/>
@@ -1353,7 +1398,7 @@
     </row>
     <row r="28" spans="1:23">
       <c r="A28" s="9" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B28" s="5"/>
       <c r="D28" s="5"/>
@@ -1377,7 +1422,7 @@
     </row>
     <row r="29" spans="1:23">
       <c r="A29" s="9" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B29" s="5"/>
       <c r="D29" s="5"/>
@@ -1401,7 +1446,7 @@
     </row>
     <row r="30" spans="1:23">
       <c r="A30" s="9" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B30" s="5"/>
       <c r="D30" s="5"/>
@@ -1425,7 +1470,7 @@
     </row>
     <row r="31" spans="1:23">
       <c r="A31" s="9" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B31" s="5"/>
       <c r="D31" s="5"/>
@@ -1449,7 +1494,7 @@
     </row>
     <row r="32" spans="1:23">
       <c r="A32" s="9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B32" s="5"/>
       <c r="D32" s="5"/>
@@ -1468,12 +1513,12 @@
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
+      <c r="V32" s="1"/>
       <c r="W32" s="7"/>
     </row>
     <row r="33" spans="1:23">
       <c r="A33" s="9" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B33" s="5"/>
       <c r="D33" s="5"/>
@@ -1497,7 +1542,7 @@
     </row>
     <row r="34" spans="1:23">
       <c r="A34" s="9" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B34" s="5"/>
       <c r="D34" s="5"/>
@@ -1521,7 +1566,7 @@
     </row>
     <row r="35" spans="1:23">
       <c r="A35" s="9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B35" s="5"/>
       <c r="D35" s="5"/>
@@ -1545,7 +1590,7 @@
     </row>
     <row r="36" spans="1:23">
       <c r="A36" s="9" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B36" s="5"/>
       <c r="D36" s="5"/>
@@ -1569,7 +1614,7 @@
     </row>
     <row r="37" spans="1:23">
       <c r="A37" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B37" s="5"/>
       <c r="D37" s="5"/>
@@ -1593,7 +1638,7 @@
     </row>
     <row r="38" spans="1:23">
       <c r="A38" s="9" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B38" s="5"/>
       <c r="D38" s="5"/>
@@ -1612,12 +1657,12 @@
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
       <c r="U38" s="5"/>
-      <c r="V38" s="1"/>
+      <c r="V38" s="5"/>
       <c r="W38" s="7"/>
     </row>
     <row r="39" spans="1:23">
-      <c r="A39" s="11" t="s">
-        <v>41</v>
+      <c r="A39" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="B39" s="5"/>
       <c r="D39" s="5"/>
@@ -1640,8 +1685,8 @@
       <c r="W39" s="7"/>
     </row>
     <row r="40" spans="1:23">
-      <c r="A40" s="12" t="s">
-        <v>42</v>
+      <c r="A40" s="11" t="s">
+        <v>39</v>
       </c>
       <c r="B40" s="5"/>
       <c r="D40" s="5"/>
@@ -1665,7 +1710,7 @@
     </row>
     <row r="41" spans="1:23">
       <c r="A41" s="12" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="B41" s="5"/>
       <c r="D41" s="5"/>
@@ -1689,7 +1734,7 @@
     </row>
     <row r="42" spans="1:23">
       <c r="A42" s="12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B42" s="5"/>
       <c r="D42" s="5"/>
@@ -1713,7 +1758,7 @@
     </row>
     <row r="43" spans="1:23">
       <c r="A43" s="12" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="B43" s="5"/>
       <c r="D43" s="5"/>
@@ -1737,7 +1782,7 @@
     </row>
     <row r="44" spans="1:23">
       <c r="A44" s="12" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="B44" s="5"/>
       <c r="D44" s="5"/>
@@ -1761,7 +1806,7 @@
     </row>
     <row r="45" spans="1:23">
       <c r="A45" s="12" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B45" s="5"/>
       <c r="D45" s="5"/>
@@ -1785,7 +1830,7 @@
     </row>
     <row r="46" spans="1:23">
       <c r="A46" s="12" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="B46" s="5"/>
       <c r="D46" s="5"/>
@@ -1809,7 +1854,7 @@
     </row>
     <row r="47" spans="1:23">
       <c r="A47" s="12" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B47" s="5"/>
       <c r="D47" s="5"/>
@@ -1833,7 +1878,7 @@
     </row>
     <row r="48" spans="1:23">
       <c r="A48" s="12" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B48" s="5"/>
       <c r="D48" s="5"/>
@@ -1857,7 +1902,7 @@
     </row>
     <row r="49" spans="1:23">
       <c r="A49" s="12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B49" s="5"/>
       <c r="D49" s="5"/>
@@ -1881,7 +1926,7 @@
     </row>
     <row r="50" spans="1:23">
       <c r="A50" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B50" s="5"/>
       <c r="D50" s="5"/>
@@ -1900,12 +1945,12 @@
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
       <c r="U50" s="5"/>
-      <c r="V50" s="5"/>
+      <c r="V50" s="1"/>
       <c r="W50" s="7"/>
     </row>
     <row r="51" spans="1:23">
       <c r="A51" s="12" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B51" s="5"/>
       <c r="D51" s="5"/>
@@ -1924,12 +1969,12 @@
       <c r="S51" s="5"/>
       <c r="T51" s="5"/>
       <c r="U51" s="5"/>
-      <c r="V51" s="5"/>
+      <c r="V51" s="1"/>
       <c r="W51" s="7"/>
     </row>
     <row r="52" spans="1:23">
       <c r="A52" s="12" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B52" s="5"/>
       <c r="D52" s="5"/>
@@ -1948,12 +1993,12 @@
       <c r="S52" s="5"/>
       <c r="T52" s="5"/>
       <c r="U52" s="5"/>
-      <c r="V52" s="5"/>
+      <c r="V52" s="1"/>
       <c r="W52" s="7"/>
     </row>
     <row r="53" spans="1:23">
       <c r="A53" s="12" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="B53" s="5"/>
       <c r="D53" s="5"/>
@@ -1972,12 +2017,12 @@
       <c r="S53" s="5"/>
       <c r="T53" s="5"/>
       <c r="U53" s="5"/>
-      <c r="V53" s="5"/>
+      <c r="V53" s="1"/>
       <c r="W53" s="7"/>
     </row>
     <row r="54" spans="1:23">
       <c r="A54" s="12" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B54" s="5"/>
       <c r="D54" s="5"/>
@@ -2001,7 +2046,7 @@
     </row>
     <row r="55" spans="1:23">
       <c r="A55" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B55" s="5"/>
       <c r="D55" s="5"/>
@@ -2025,7 +2070,7 @@
     </row>
     <row r="56" spans="1:23">
       <c r="A56" s="12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B56" s="5"/>
       <c r="D56" s="5"/>
@@ -2048,8 +2093,8 @@
       <c r="W56" s="7"/>
     </row>
     <row r="57" spans="1:23">
-      <c r="A57" s="13" t="s">
-        <v>71</v>
+      <c r="A57" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="B57" s="5"/>
       <c r="D57" s="5"/>
@@ -2073,7 +2118,7 @@
     </row>
     <row r="58" spans="1:23">
       <c r="A58" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B58" s="5"/>
       <c r="D58" s="5"/>
@@ -2097,7 +2142,7 @@
     </row>
     <row r="59" spans="1:23">
       <c r="A59" s="12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B59" s="5"/>
       <c r="D59" s="5"/>
@@ -2121,7 +2166,7 @@
     </row>
     <row r="60" spans="1:23">
       <c r="A60" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B60" s="5"/>
       <c r="D60" s="5"/>
@@ -2144,8 +2189,8 @@
       <c r="W60" s="7"/>
     </row>
     <row r="61" spans="1:23">
-      <c r="A61" s="12" t="s">
-        <v>57</v>
+      <c r="A61" s="13" t="s">
+        <v>67</v>
       </c>
       <c r="B61" s="5"/>
       <c r="D61" s="5"/>
@@ -2169,7 +2214,7 @@
     </row>
     <row r="62" spans="1:23">
       <c r="A62" s="12" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B62" s="5"/>
       <c r="D62" s="5"/>
@@ -2193,7 +2238,7 @@
     </row>
     <row r="63" spans="1:23">
       <c r="A63" s="12" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B63" s="5"/>
       <c r="D63" s="5"/>
@@ -2217,7 +2262,7 @@
     </row>
     <row r="64" spans="1:23">
       <c r="A64" s="12" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B64" s="5"/>
       <c r="D64" s="5"/>
@@ -2241,7 +2286,7 @@
     </row>
     <row r="65" spans="1:23">
       <c r="A65" s="12" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B65" s="5"/>
       <c r="D65" s="5"/>
@@ -2265,7 +2310,7 @@
     </row>
     <row r="66" spans="1:23">
       <c r="A66" s="12" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B66" s="5"/>
       <c r="D66" s="5"/>
@@ -2284,12 +2329,12 @@
       <c r="S66" s="5"/>
       <c r="T66" s="5"/>
       <c r="U66" s="5"/>
-      <c r="V66" s="1"/>
+      <c r="V66" s="5"/>
       <c r="W66" s="7"/>
     </row>
     <row r="67" spans="1:23">
       <c r="A67" s="12" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B67" s="5"/>
       <c r="D67" s="5"/>
@@ -2308,12 +2353,12 @@
       <c r="S67" s="5"/>
       <c r="T67" s="5"/>
       <c r="U67" s="5"/>
-      <c r="V67" s="1"/>
+      <c r="V67" s="5"/>
       <c r="W67" s="7"/>
     </row>
     <row r="68" spans="1:23">
       <c r="A68" s="12" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="B68" s="5"/>
       <c r="D68" s="5"/>
@@ -2332,12 +2377,12 @@
       <c r="S68" s="5"/>
       <c r="T68" s="5"/>
       <c r="U68" s="5"/>
-      <c r="V68" s="1"/>
+      <c r="V68" s="5"/>
       <c r="W68" s="7"/>
     </row>
     <row r="69" spans="1:23">
       <c r="A69" s="12" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="B69" s="5"/>
       <c r="D69" s="5"/>
@@ -2356,12 +2401,12 @@
       <c r="S69" s="5"/>
       <c r="T69" s="5"/>
       <c r="U69" s="5"/>
-      <c r="V69" s="1"/>
+      <c r="V69" s="5"/>
       <c r="W69" s="7"/>
     </row>
     <row r="70" spans="1:23">
       <c r="A70" s="12" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B70" s="5"/>
       <c r="D70" s="5"/>
@@ -2385,7 +2430,7 @@
     </row>
     <row r="71" spans="1:23">
       <c r="A71" s="12" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B71" s="5"/>
       <c r="D71" s="5"/>
@@ -2409,7 +2454,7 @@
     </row>
     <row r="72" spans="1:23">
       <c r="A72" s="12" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B72" s="5"/>
       <c r="D72" s="5"/>
@@ -2428,12 +2473,12 @@
       <c r="S72" s="5"/>
       <c r="T72" s="5"/>
       <c r="U72" s="5"/>
-      <c r="V72" s="1"/>
+      <c r="V72" s="5"/>
       <c r="W72" s="7"/>
     </row>
     <row r="73" spans="1:23">
       <c r="A73" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B73" s="5"/>
       <c r="D73" s="5"/>
@@ -2452,12 +2497,12 @@
       <c r="S73" s="5"/>
       <c r="T73" s="5"/>
       <c r="U73" s="5"/>
-      <c r="V73" s="1"/>
+      <c r="V73" s="5"/>
       <c r="W73" s="7"/>
     </row>
     <row r="74" spans="1:23">
       <c r="A74" s="12" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B74" s="5"/>
       <c r="D74" s="5"/>
@@ -2481,7 +2526,7 @@
     </row>
     <row r="75" spans="1:23">
       <c r="A75" s="12" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B75" s="5"/>
       <c r="D75" s="5"/>
@@ -2505,7 +2550,7 @@
     </row>
     <row r="76" spans="1:23">
       <c r="A76" s="12" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B76" s="5"/>
       <c r="D76" s="5"/>
@@ -2524,10 +2569,13 @@
       <c r="S76" s="5"/>
       <c r="T76" s="5"/>
       <c r="U76" s="5"/>
-      <c r="V76" s="5"/>
+      <c r="V76" s="1"/>
       <c r="W76" s="7"/>
     </row>
     <row r="77" spans="1:23">
+      <c r="A77" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="B77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
@@ -2545,10 +2593,13 @@
       <c r="S77" s="5"/>
       <c r="T77" s="5"/>
       <c r="U77" s="5"/>
-      <c r="V77" s="5"/>
+      <c r="V77" s="1"/>
       <c r="W77" s="7"/>
     </row>
     <row r="78" spans="1:23">
+      <c r="A78" s="12" t="s">
+        <v>62</v>
+      </c>
       <c r="B78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
@@ -2570,6 +2621,9 @@
       <c r="W78" s="7"/>
     </row>
     <row r="79" spans="1:23">
+      <c r="A79" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="B79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
@@ -2591,6 +2645,9 @@
       <c r="W79" s="7"/>
     </row>
     <row r="80" spans="1:23">
+      <c r="A80" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="B80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
@@ -2608,10 +2665,13 @@
       <c r="S80" s="5"/>
       <c r="T80" s="5"/>
       <c r="U80" s="5"/>
-      <c r="V80" s="5"/>
+      <c r="V80" s="1"/>
       <c r="W80" s="7"/>
     </row>
     <row r="81" spans="1:23">
+      <c r="A81" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="B81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
@@ -2629,10 +2689,13 @@
       <c r="S81" s="5"/>
       <c r="T81" s="5"/>
       <c r="U81" s="5"/>
-      <c r="V81" s="5"/>
+      <c r="V81" s="1"/>
       <c r="W81" s="7"/>
     </row>
     <row r="82" spans="1:23">
+      <c r="A82" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="B82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
@@ -2650,10 +2713,13 @@
       <c r="S82" s="5"/>
       <c r="T82" s="5"/>
       <c r="U82" s="5"/>
-      <c r="V82" s="5"/>
+      <c r="V82" s="1"/>
       <c r="W82" s="7"/>
     </row>
     <row r="83" spans="1:23">
+      <c r="A83" s="12" t="s">
+        <v>66</v>
+      </c>
       <c r="B83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
@@ -2671,10 +2737,13 @@
       <c r="S83" s="5"/>
       <c r="T83" s="5"/>
       <c r="U83" s="5"/>
-      <c r="V83" s="5"/>
+      <c r="V83" s="1"/>
       <c r="W83" s="7"/>
     </row>
     <row r="84" spans="1:23">
+      <c r="A84" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="B84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
@@ -2692,10 +2761,13 @@
       <c r="S84" s="5"/>
       <c r="T84" s="5"/>
       <c r="U84" s="5"/>
-      <c r="V84" s="5"/>
+      <c r="V84" s="1"/>
       <c r="W84" s="7"/>
     </row>
     <row r="85" spans="1:23">
+      <c r="A85" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="B85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
@@ -2717,6 +2789,9 @@
       <c r="W85" s="7"/>
     </row>
     <row r="86" spans="1:23">
+      <c r="A86" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="B86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
@@ -2738,8 +2813,10 @@
       <c r="W86" s="7"/>
     </row>
     <row r="87" spans="1:23">
+      <c r="A87" s="12" t="s">
+        <v>78</v>
+      </c>
       <c r="B87" s="5"/>
-      <c r="C87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
       <c r="H87" s="5"/>
@@ -2760,8 +2837,10 @@
       <c r="W87" s="7"/>
     </row>
     <row r="88" spans="1:23">
+      <c r="A88" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="B88" s="5"/>
-      <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
       <c r="H88" s="5"/>
@@ -2782,9 +2861,10 @@
       <c r="W88" s="7"/>
     </row>
     <row r="89" spans="1:23">
-      <c r="A89" s="3"/>
+      <c r="A89" s="12" t="s">
+        <v>82</v>
+      </c>
       <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
       <c r="H89" s="5"/>
@@ -2805,9 +2885,10 @@
       <c r="W89" s="7"/>
     </row>
     <row r="90" spans="1:23">
-      <c r="A90" s="3"/>
+      <c r="A90" s="12" t="s">
+        <v>83</v>
+      </c>
       <c r="B90" s="5"/>
-      <c r="C90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
       <c r="H90" s="5"/>
@@ -2828,9 +2909,10 @@
       <c r="W90" s="7"/>
     </row>
     <row r="91" spans="1:23">
-      <c r="A91" s="3"/>
+      <c r="A91" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
       <c r="H91" s="5"/>
@@ -2851,9 +2933,7 @@
       <c r="W91" s="7"/>
     </row>
     <row r="92" spans="1:23">
-      <c r="A92" s="3"/>
       <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
       <c r="H92" s="5"/>
@@ -2870,13 +2950,11 @@
       <c r="S92" s="5"/>
       <c r="T92" s="5"/>
       <c r="U92" s="5"/>
-      <c r="V92" s="1"/>
+      <c r="V92" s="5"/>
       <c r="W92" s="7"/>
     </row>
     <row r="93" spans="1:23">
-      <c r="A93" s="3"/>
       <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
       <c r="H93" s="5"/>
@@ -2893,13 +2971,11 @@
       <c r="S93" s="5"/>
       <c r="T93" s="5"/>
       <c r="U93" s="5"/>
-      <c r="V93" s="1"/>
+      <c r="V93" s="5"/>
       <c r="W93" s="7"/>
     </row>
     <row r="94" spans="1:23">
-      <c r="A94" s="3"/>
       <c r="B94" s="5"/>
-      <c r="C94" s="5"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
       <c r="H94" s="5"/>
@@ -2920,9 +2996,7 @@
       <c r="W94" s="7"/>
     </row>
     <row r="95" spans="1:23">
-      <c r="A95" s="3"/>
       <c r="B95" s="5"/>
-      <c r="C95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
       <c r="H95" s="5"/>
@@ -2943,7 +3017,6 @@
       <c r="W95" s="7"/>
     </row>
     <row r="96" spans="1:23">
-      <c r="A96" s="3"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -2966,7 +3039,6 @@
       <c r="W96" s="7"/>
     </row>
     <row r="97" spans="1:23">
-      <c r="A97" s="3"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -3054,7 +3126,7 @@
       <c r="S100" s="5"/>
       <c r="T100" s="5"/>
       <c r="U100" s="5"/>
-      <c r="V100" s="1"/>
+      <c r="V100" s="5"/>
       <c r="W100" s="7"/>
     </row>
     <row r="101" spans="1:23">
@@ -3081,6 +3153,7 @@
       <c r="W101" s="7"/>
     </row>
     <row r="102" spans="1:23">
+      <c r="A102" s="3"/>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
@@ -3099,10 +3172,11 @@
       <c r="S102" s="5"/>
       <c r="T102" s="5"/>
       <c r="U102" s="5"/>
-      <c r="V102" s="5"/>
+      <c r="V102" s="1"/>
       <c r="W102" s="7"/>
     </row>
     <row r="103" spans="1:23">
+      <c r="A103" s="3"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
@@ -3125,6 +3199,7 @@
       <c r="W103" s="7"/>
     </row>
     <row r="104" spans="1:23">
+      <c r="A104" s="3"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
@@ -3147,6 +3222,7 @@
       <c r="W104" s="7"/>
     </row>
     <row r="105" spans="1:23">
+      <c r="A105" s="3"/>
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -3169,6 +3245,7 @@
       <c r="W105" s="7"/>
     </row>
     <row r="106" spans="1:23">
+      <c r="A106" s="3"/>
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
@@ -3191,6 +3268,7 @@
       <c r="W106" s="7"/>
     </row>
     <row r="107" spans="1:23">
+      <c r="A107" s="3"/>
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
@@ -3213,6 +3291,7 @@
       <c r="W107" s="7"/>
     </row>
     <row r="108" spans="1:23">
+      <c r="A108" s="3"/>
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
@@ -3235,6 +3314,7 @@
       <c r="W108" s="7"/>
     </row>
     <row r="109" spans="1:23">
+      <c r="A109" s="3"/>
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -3253,10 +3333,11 @@
       <c r="S109" s="5"/>
       <c r="T109" s="5"/>
       <c r="U109" s="5"/>
-      <c r="V109" s="5"/>
+      <c r="V109" s="1"/>
       <c r="W109" s="7"/>
     </row>
     <row r="110" spans="1:23">
+      <c r="A110" s="3"/>
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
@@ -3297,7 +3378,7 @@
       <c r="S111" s="5"/>
       <c r="T111" s="5"/>
       <c r="U111" s="5"/>
-      <c r="V111" s="1"/>
+      <c r="V111" s="5"/>
       <c r="W111" s="7"/>
     </row>
     <row r="112" spans="1:23">
@@ -3319,7 +3400,7 @@
       <c r="S112" s="5"/>
       <c r="T112" s="5"/>
       <c r="U112" s="5"/>
-      <c r="V112" s="1"/>
+      <c r="V112" s="5"/>
       <c r="W112" s="7"/>
     </row>
     <row r="113" spans="1:23">
@@ -3341,7 +3422,7 @@
       <c r="S113" s="5"/>
       <c r="T113" s="5"/>
       <c r="U113" s="5"/>
-      <c r="V113" s="1"/>
+      <c r="V113" s="5"/>
       <c r="W113" s="7"/>
     </row>
     <row r="114" spans="1:23">
@@ -3363,11 +3444,10 @@
       <c r="S114" s="5"/>
       <c r="T114" s="5"/>
       <c r="U114" s="5"/>
-      <c r="V114" s="1"/>
+      <c r="V114" s="5"/>
       <c r="W114" s="7"/>
     </row>
     <row r="115" spans="1:23">
-      <c r="A115" s="3"/>
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
@@ -3386,7 +3466,7 @@
       <c r="S115" s="5"/>
       <c r="T115" s="5"/>
       <c r="U115" s="5"/>
-      <c r="V115" s="1"/>
+      <c r="V115" s="5"/>
       <c r="W115" s="7"/>
     </row>
     <row r="116" spans="1:23">
@@ -3408,7 +3488,7 @@
       <c r="S116" s="5"/>
       <c r="T116" s="5"/>
       <c r="U116" s="5"/>
-      <c r="V116" s="1"/>
+      <c r="V116" s="5"/>
       <c r="W116" s="7"/>
     </row>
     <row r="117" spans="1:23">
@@ -3430,7 +3510,7 @@
       <c r="S117" s="5"/>
       <c r="T117" s="5"/>
       <c r="U117" s="5"/>
-      <c r="V117" s="1"/>
+      <c r="V117" s="5"/>
       <c r="W117" s="7"/>
     </row>
     <row r="118" spans="1:23">
@@ -3452,7 +3532,7 @@
       <c r="S118" s="5"/>
       <c r="T118" s="5"/>
       <c r="U118" s="5"/>
-      <c r="V118" s="1"/>
+      <c r="V118" s="5"/>
       <c r="W118" s="7"/>
     </row>
     <row r="119" spans="1:23">
@@ -3496,7 +3576,7 @@
       <c r="S120" s="5"/>
       <c r="T120" s="5"/>
       <c r="U120" s="5"/>
-      <c r="V120" s="5"/>
+      <c r="V120" s="1"/>
       <c r="W120" s="7"/>
     </row>
     <row r="121" spans="1:23">
@@ -3518,11 +3598,10 @@
       <c r="S121" s="5"/>
       <c r="T121" s="5"/>
       <c r="U121" s="5"/>
-      <c r="V121" s="5"/>
+      <c r="V121" s="1"/>
       <c r="W121" s="7"/>
     </row>
     <row r="122" spans="1:23">
-      <c r="A122" s="3"/>
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
@@ -3563,7 +3642,7 @@
       <c r="S123" s="5"/>
       <c r="T123" s="5"/>
       <c r="U123" s="5"/>
-      <c r="V123" s="5"/>
+      <c r="V123" s="1"/>
       <c r="W123" s="7"/>
     </row>
     <row r="124" spans="1:23">
@@ -3586,7 +3665,7 @@
       <c r="S124" s="5"/>
       <c r="T124" s="5"/>
       <c r="U124" s="5"/>
-      <c r="V124" s="5"/>
+      <c r="V124" s="1"/>
       <c r="W124" s="7"/>
     </row>
     <row r="125" spans="1:23">
@@ -3677,7 +3756,7 @@
       <c r="V128" s="1"/>
       <c r="W128" s="7"/>
     </row>
-    <row r="129" spans="2:23">
+    <row r="129" spans="1:23">
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
@@ -3696,10 +3775,10 @@
       <c r="S129" s="5"/>
       <c r="T129" s="5"/>
       <c r="U129" s="5"/>
-      <c r="V129" s="1"/>
+      <c r="V129" s="5"/>
       <c r="W129" s="7"/>
     </row>
-    <row r="130" spans="2:23">
+    <row r="130" spans="1:23">
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
@@ -3718,10 +3797,11 @@
       <c r="S130" s="5"/>
       <c r="T130" s="5"/>
       <c r="U130" s="5"/>
-      <c r="V130" s="1"/>
+      <c r="V130" s="5"/>
       <c r="W130" s="7"/>
     </row>
-    <row r="131" spans="2:23">
+    <row r="131" spans="1:23">
+      <c r="A131" s="3"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
@@ -3743,7 +3823,7 @@
       <c r="V131" s="1"/>
       <c r="W131" s="7"/>
     </row>
-    <row r="132" spans="2:23">
+    <row r="132" spans="1:23">
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
@@ -3762,10 +3842,11 @@
       <c r="S132" s="5"/>
       <c r="T132" s="5"/>
       <c r="U132" s="5"/>
-      <c r="V132" s="1"/>
+      <c r="V132" s="5"/>
       <c r="W132" s="7"/>
     </row>
-    <row r="133" spans="2:23">
+    <row r="133" spans="1:23">
+      <c r="A133" s="3"/>
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
@@ -3784,10 +3865,10 @@
       <c r="S133" s="5"/>
       <c r="T133" s="5"/>
       <c r="U133" s="5"/>
-      <c r="V133" s="1"/>
+      <c r="V133" s="5"/>
       <c r="W133" s="7"/>
     </row>
-    <row r="134" spans="2:23">
+    <row r="134" spans="1:23">
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
@@ -3806,10 +3887,10 @@
       <c r="S134" s="5"/>
       <c r="T134" s="5"/>
       <c r="U134" s="5"/>
-      <c r="V134" s="5"/>
+      <c r="V134" s="1"/>
       <c r="W134" s="7"/>
     </row>
-    <row r="135" spans="2:23">
+    <row r="135" spans="1:23">
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
@@ -3828,10 +3909,10 @@
       <c r="S135" s="5"/>
       <c r="T135" s="5"/>
       <c r="U135" s="5"/>
-      <c r="V135" s="5"/>
+      <c r="V135" s="1"/>
       <c r="W135" s="7"/>
     </row>
-    <row r="136" spans="2:23">
+    <row r="136" spans="1:23">
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
@@ -3853,7 +3934,7 @@
       <c r="V136" s="1"/>
       <c r="W136" s="7"/>
     </row>
-    <row r="137" spans="2:23">
+    <row r="137" spans="1:23">
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
@@ -3872,10 +3953,10 @@
       <c r="S137" s="5"/>
       <c r="T137" s="5"/>
       <c r="U137" s="5"/>
-      <c r="V137" s="5"/>
+      <c r="V137" s="1"/>
       <c r="W137" s="7"/>
     </row>
-    <row r="138" spans="2:23">
+    <row r="138" spans="1:23">
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
       <c r="D138" s="5"/>
@@ -3894,10 +3975,10 @@
       <c r="S138" s="5"/>
       <c r="T138" s="5"/>
       <c r="U138" s="5"/>
-      <c r="V138" s="5"/>
+      <c r="V138" s="1"/>
       <c r="W138" s="7"/>
     </row>
-    <row r="139" spans="2:23">
+    <row r="139" spans="1:23">
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
@@ -3916,10 +3997,10 @@
       <c r="S139" s="5"/>
       <c r="T139" s="5"/>
       <c r="U139" s="5"/>
-      <c r="V139" s="5"/>
+      <c r="V139" s="1"/>
       <c r="W139" s="7"/>
     </row>
-    <row r="140" spans="2:23">
+    <row r="140" spans="1:23">
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
@@ -3941,7 +4022,7 @@
       <c r="V140" s="1"/>
       <c r="W140" s="7"/>
     </row>
-    <row r="141" spans="2:23">
+    <row r="141" spans="1:23">
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
       <c r="D141" s="5"/>
@@ -3963,7 +4044,7 @@
       <c r="V141" s="1"/>
       <c r="W141" s="7"/>
     </row>
-    <row r="142" spans="2:23">
+    <row r="142" spans="1:23">
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
       <c r="D142" s="5"/>
@@ -3982,10 +4063,10 @@
       <c r="S142" s="5"/>
       <c r="T142" s="5"/>
       <c r="U142" s="5"/>
-      <c r="V142" s="5"/>
+      <c r="V142" s="1"/>
       <c r="W142" s="7"/>
     </row>
-    <row r="143" spans="2:23">
+    <row r="143" spans="1:23">
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
@@ -4007,7 +4088,7 @@
       <c r="V143" s="5"/>
       <c r="W143" s="7"/>
     </row>
-    <row r="144" spans="2:23">
+    <row r="144" spans="1:23">
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
       <c r="D144" s="5"/>
@@ -4048,7 +4129,7 @@
       <c r="S145" s="5"/>
       <c r="T145" s="5"/>
       <c r="U145" s="5"/>
-      <c r="V145" s="5"/>
+      <c r="V145" s="1"/>
       <c r="W145" s="7"/>
     </row>
     <row r="146" spans="2:23">
@@ -4136,7 +4217,7 @@
       <c r="S149" s="5"/>
       <c r="T149" s="5"/>
       <c r="U149" s="5"/>
-      <c r="V149" s="5"/>
+      <c r="V149" s="1"/>
       <c r="W149" s="7"/>
     </row>
     <row r="150" spans="2:23">
@@ -4158,7 +4239,7 @@
       <c r="S150" s="5"/>
       <c r="T150" s="5"/>
       <c r="U150" s="5"/>
-      <c r="V150" s="5"/>
+      <c r="V150" s="1"/>
       <c r="W150" s="7"/>
     </row>
     <row r="151" spans="2:23">
@@ -4334,7 +4415,7 @@
       <c r="S158" s="5"/>
       <c r="T158" s="5"/>
       <c r="U158" s="5"/>
-      <c r="V158" s="1"/>
+      <c r="V158" s="5"/>
       <c r="W158" s="7"/>
     </row>
     <row r="159" spans="2:23">
@@ -4356,7 +4437,7 @@
       <c r="S159" s="5"/>
       <c r="T159" s="5"/>
       <c r="U159" s="5"/>
-      <c r="V159" s="1"/>
+      <c r="V159" s="5"/>
       <c r="W159" s="7"/>
     </row>
     <row r="160" spans="2:23">
@@ -4422,7 +4503,7 @@
       <c r="S162" s="5"/>
       <c r="T162" s="5"/>
       <c r="U162" s="5"/>
-      <c r="V162" s="1"/>
+      <c r="V162" s="5"/>
       <c r="W162" s="7"/>
     </row>
     <row r="163" spans="2:23">
@@ -4444,7 +4525,7 @@
       <c r="S163" s="5"/>
       <c r="T163" s="5"/>
       <c r="U163" s="5"/>
-      <c r="V163" s="1"/>
+      <c r="V163" s="5"/>
       <c r="W163" s="7"/>
     </row>
     <row r="164" spans="2:23">
@@ -4532,7 +4613,7 @@
       <c r="S167" s="5"/>
       <c r="T167" s="5"/>
       <c r="U167" s="5"/>
-      <c r="V167" s="5"/>
+      <c r="V167" s="1"/>
       <c r="W167" s="7"/>
     </row>
     <row r="168" spans="2:23">
@@ -4554,7 +4635,7 @@
       <c r="S168" s="5"/>
       <c r="T168" s="5"/>
       <c r="U168" s="5"/>
-      <c r="V168" s="5"/>
+      <c r="V168" s="1"/>
       <c r="W168" s="7"/>
     </row>
     <row r="169" spans="2:23">
@@ -4620,7 +4701,7 @@
       <c r="S171" s="5"/>
       <c r="T171" s="5"/>
       <c r="U171" s="5"/>
-      <c r="V171" s="5"/>
+      <c r="V171" s="1"/>
       <c r="W171" s="7"/>
     </row>
     <row r="172" spans="2:23">
@@ -4642,7 +4723,7 @@
       <c r="S172" s="5"/>
       <c r="T172" s="5"/>
       <c r="U172" s="5"/>
-      <c r="V172" s="5"/>
+      <c r="V172" s="1"/>
       <c r="W172" s="7"/>
     </row>
     <row r="173" spans="2:23">
@@ -4818,7 +4899,7 @@
       <c r="S180" s="5"/>
       <c r="T180" s="5"/>
       <c r="U180" s="5"/>
-      <c r="V180" s="1"/>
+      <c r="V180" s="5"/>
       <c r="W180" s="7"/>
     </row>
     <row r="181" spans="2:23">
@@ -4840,7 +4921,7 @@
       <c r="S181" s="5"/>
       <c r="T181" s="5"/>
       <c r="U181" s="5"/>
-      <c r="V181" s="1"/>
+      <c r="V181" s="5"/>
       <c r="W181" s="7"/>
     </row>
     <row r="182" spans="2:23">
@@ -4862,7 +4943,7 @@
       <c r="S182" s="5"/>
       <c r="T182" s="5"/>
       <c r="U182" s="5"/>
-      <c r="V182" s="1"/>
+      <c r="V182" s="5"/>
       <c r="W182" s="7"/>
     </row>
     <row r="183" spans="2:23">
@@ -4884,7 +4965,7 @@
       <c r="S183" s="5"/>
       <c r="T183" s="5"/>
       <c r="U183" s="5"/>
-      <c r="V183" s="1"/>
+      <c r="V183" s="5"/>
       <c r="W183" s="7"/>
     </row>
     <row r="184" spans="2:23">
@@ -4994,7 +5075,7 @@
       <c r="S188" s="5"/>
       <c r="T188" s="5"/>
       <c r="U188" s="5"/>
-      <c r="V188" s="1"/>
+      <c r="V188" s="5"/>
       <c r="W188" s="7"/>
     </row>
     <row r="189" spans="2:23">
@@ -5038,7 +5119,7 @@
       <c r="S190" s="5"/>
       <c r="T190" s="5"/>
       <c r="U190" s="5"/>
-      <c r="V190" s="5"/>
+      <c r="V190" s="1"/>
       <c r="W190" s="7"/>
     </row>
     <row r="191" spans="2:23">
@@ -5060,7 +5141,7 @@
       <c r="S191" s="5"/>
       <c r="T191" s="5"/>
       <c r="U191" s="5"/>
-      <c r="V191" s="5"/>
+      <c r="V191" s="1"/>
       <c r="W191" s="7"/>
     </row>
     <row r="192" spans="2:23">
@@ -5082,10 +5163,10 @@
       <c r="S192" s="5"/>
       <c r="T192" s="5"/>
       <c r="U192" s="5"/>
-      <c r="V192" s="5"/>
+      <c r="V192" s="1"/>
       <c r="W192" s="7"/>
     </row>
-    <row r="193" spans="1:23">
+    <row r="193" spans="2:23">
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
@@ -5107,7 +5188,7 @@
       <c r="V193" s="5"/>
       <c r="W193" s="7"/>
     </row>
-    <row r="194" spans="1:23">
+    <row r="194" spans="2:23">
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
@@ -5129,7 +5210,7 @@
       <c r="V194" s="5"/>
       <c r="W194" s="7"/>
     </row>
-    <row r="195" spans="1:23">
+    <row r="195" spans="2:23">
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
@@ -5151,7 +5232,7 @@
       <c r="V195" s="5"/>
       <c r="W195" s="7"/>
     </row>
-    <row r="196" spans="1:23">
+    <row r="196" spans="2:23">
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
@@ -5173,7 +5254,7 @@
       <c r="V196" s="5"/>
       <c r="W196" s="7"/>
     </row>
-    <row r="197" spans="1:23">
+    <row r="197" spans="2:23">
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
@@ -5192,10 +5273,10 @@
       <c r="S197" s="5"/>
       <c r="T197" s="5"/>
       <c r="U197" s="5"/>
-      <c r="V197" s="5"/>
+      <c r="V197" s="1"/>
       <c r="W197" s="7"/>
     </row>
-    <row r="198" spans="1:23">
+    <row r="198" spans="2:23">
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
@@ -5214,10 +5295,10 @@
       <c r="S198" s="5"/>
       <c r="T198" s="5"/>
       <c r="U198" s="5"/>
-      <c r="V198" s="5"/>
+      <c r="V198" s="1"/>
       <c r="W198" s="7"/>
     </row>
-    <row r="199" spans="1:23">
+    <row r="199" spans="2:23">
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
@@ -5239,7 +5320,7 @@
       <c r="V199" s="5"/>
       <c r="W199" s="7"/>
     </row>
-    <row r="200" spans="1:23">
+    <row r="200" spans="2:23">
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
@@ -5258,10 +5339,10 @@
       <c r="S200" s="5"/>
       <c r="T200" s="5"/>
       <c r="U200" s="5"/>
-      <c r="V200" s="1"/>
+      <c r="V200" s="5"/>
       <c r="W200" s="7"/>
     </row>
-    <row r="201" spans="1:23">
+    <row r="201" spans="2:23">
       <c r="B201" s="5"/>
       <c r="C201" s="5"/>
       <c r="D201" s="5"/>
@@ -5280,11 +5361,10 @@
       <c r="S201" s="5"/>
       <c r="T201" s="5"/>
       <c r="U201" s="5"/>
-      <c r="V201" s="1"/>
+      <c r="V201" s="5"/>
       <c r="W201" s="7"/>
     </row>
-    <row r="202" spans="1:23">
-      <c r="A202" s="3"/>
+    <row r="202" spans="2:23">
       <c r="B202" s="5"/>
       <c r="C202" s="5"/>
       <c r="D202" s="5"/>
@@ -5306,7 +5386,7 @@
       <c r="V202" s="5"/>
       <c r="W202" s="7"/>
     </row>
-    <row r="203" spans="1:23">
+    <row r="203" spans="2:23">
       <c r="B203" s="5"/>
       <c r="C203" s="5"/>
       <c r="D203" s="5"/>
@@ -5328,8 +5408,7 @@
       <c r="V203" s="5"/>
       <c r="W203" s="7"/>
     </row>
-    <row r="204" spans="1:23">
-      <c r="A204" s="8"/>
+    <row r="204" spans="2:23">
       <c r="B204" s="5"/>
       <c r="C204" s="5"/>
       <c r="D204" s="5"/>
@@ -5351,8 +5430,7 @@
       <c r="V204" s="5"/>
       <c r="W204" s="7"/>
     </row>
-    <row r="205" spans="1:23">
-      <c r="A205" s="3"/>
+    <row r="205" spans="2:23">
       <c r="B205" s="5"/>
       <c r="C205" s="5"/>
       <c r="D205" s="5"/>
@@ -5374,8 +5452,7 @@
       <c r="V205" s="5"/>
       <c r="W205" s="7"/>
     </row>
-    <row r="206" spans="1:23">
-      <c r="A206" s="3"/>
+    <row r="206" spans="2:23">
       <c r="B206" s="5"/>
       <c r="C206" s="5"/>
       <c r="D206" s="5"/>
@@ -5394,10 +5471,10 @@
       <c r="S206" s="5"/>
       <c r="T206" s="5"/>
       <c r="U206" s="5"/>
-      <c r="V206" s="1"/>
+      <c r="V206" s="5"/>
       <c r="W206" s="7"/>
     </row>
-    <row r="207" spans="1:23">
+    <row r="207" spans="2:23">
       <c r="B207" s="5"/>
       <c r="C207" s="5"/>
       <c r="D207" s="5"/>
@@ -5416,10 +5493,10 @@
       <c r="S207" s="5"/>
       <c r="T207" s="5"/>
       <c r="U207" s="5"/>
-      <c r="V207" s="1"/>
+      <c r="V207" s="5"/>
       <c r="W207" s="7"/>
     </row>
-    <row r="208" spans="1:23">
+    <row r="208" spans="2:23">
       <c r="B208" s="5"/>
       <c r="C208" s="5"/>
       <c r="D208" s="5"/>
@@ -5441,7 +5518,7 @@
       <c r="V208" s="5"/>
       <c r="W208" s="7"/>
     </row>
-    <row r="209" spans="2:23">
+    <row r="209" spans="1:23">
       <c r="B209" s="5"/>
       <c r="C209" s="5"/>
       <c r="D209" s="5"/>
@@ -5460,10 +5537,10 @@
       <c r="S209" s="5"/>
       <c r="T209" s="5"/>
       <c r="U209" s="5"/>
-      <c r="V209" s="5"/>
+      <c r="V209" s="1"/>
       <c r="W209" s="7"/>
     </row>
-    <row r="210" spans="2:23">
+    <row r="210" spans="1:23">
       <c r="B210" s="5"/>
       <c r="C210" s="5"/>
       <c r="D210" s="5"/>
@@ -5482,10 +5559,11 @@
       <c r="S210" s="5"/>
       <c r="T210" s="5"/>
       <c r="U210" s="5"/>
-      <c r="V210" s="5"/>
+      <c r="V210" s="1"/>
       <c r="W210" s="7"/>
     </row>
-    <row r="211" spans="2:23">
+    <row r="211" spans="1:23">
+      <c r="A211" s="3"/>
       <c r="B211" s="5"/>
       <c r="C211" s="5"/>
       <c r="D211" s="5"/>
@@ -5507,7 +5585,7 @@
       <c r="V211" s="5"/>
       <c r="W211" s="7"/>
     </row>
-    <row r="212" spans="2:23">
+    <row r="212" spans="1:23">
       <c r="B212" s="5"/>
       <c r="C212" s="5"/>
       <c r="D212" s="5"/>
@@ -5529,7 +5607,8 @@
       <c r="V212" s="5"/>
       <c r="W212" s="7"/>
     </row>
-    <row r="213" spans="2:23">
+    <row r="213" spans="1:23">
+      <c r="A213" s="8"/>
       <c r="B213" s="5"/>
       <c r="C213" s="5"/>
       <c r="D213" s="5"/>
@@ -5551,7 +5630,8 @@
       <c r="V213" s="5"/>
       <c r="W213" s="7"/>
     </row>
-    <row r="214" spans="2:23">
+    <row r="214" spans="1:23">
+      <c r="A214" s="3"/>
       <c r="B214" s="5"/>
       <c r="C214" s="5"/>
       <c r="D214" s="5"/>
@@ -5573,7 +5653,8 @@
       <c r="V214" s="5"/>
       <c r="W214" s="7"/>
     </row>
-    <row r="215" spans="2:23">
+    <row r="215" spans="1:23">
+      <c r="A215" s="3"/>
       <c r="B215" s="5"/>
       <c r="C215" s="5"/>
       <c r="D215" s="5"/>
@@ -5592,10 +5673,10 @@
       <c r="S215" s="5"/>
       <c r="T215" s="5"/>
       <c r="U215" s="5"/>
-      <c r="V215" s="5"/>
+      <c r="V215" s="1"/>
       <c r="W215" s="7"/>
     </row>
-    <row r="216" spans="2:23">
+    <row r="216" spans="1:23">
       <c r="B216" s="5"/>
       <c r="C216" s="5"/>
       <c r="D216" s="5"/>
@@ -5614,10 +5695,10 @@
       <c r="S216" s="5"/>
       <c r="T216" s="5"/>
       <c r="U216" s="5"/>
-      <c r="V216" s="5"/>
+      <c r="V216" s="1"/>
       <c r="W216" s="7"/>
     </row>
-    <row r="217" spans="2:23">
+    <row r="217" spans="1:23">
       <c r="B217" s="5"/>
       <c r="C217" s="5"/>
       <c r="D217" s="5"/>
@@ -5639,7 +5720,7 @@
       <c r="V217" s="5"/>
       <c r="W217" s="7"/>
     </row>
-    <row r="218" spans="2:23">
+    <row r="218" spans="1:23">
       <c r="B218" s="5"/>
       <c r="C218" s="5"/>
       <c r="D218" s="5"/>
@@ -5661,7 +5742,7 @@
       <c r="V218" s="5"/>
       <c r="W218" s="7"/>
     </row>
-    <row r="219" spans="2:23">
+    <row r="219" spans="1:23">
       <c r="B219" s="5"/>
       <c r="C219" s="5"/>
       <c r="D219" s="5"/>
@@ -5683,7 +5764,7 @@
       <c r="V219" s="5"/>
       <c r="W219" s="7"/>
     </row>
-    <row r="220" spans="2:23">
+    <row r="220" spans="1:23">
       <c r="B220" s="5"/>
       <c r="C220" s="5"/>
       <c r="D220" s="5"/>
@@ -5705,7 +5786,7 @@
       <c r="V220" s="5"/>
       <c r="W220" s="7"/>
     </row>
-    <row r="221" spans="2:23">
+    <row r="221" spans="1:23">
       <c r="B221" s="5"/>
       <c r="C221" s="5"/>
       <c r="D221" s="5"/>
@@ -5727,7 +5808,7 @@
       <c r="V221" s="5"/>
       <c r="W221" s="7"/>
     </row>
-    <row r="222" spans="2:23">
+    <row r="222" spans="1:23">
       <c r="B222" s="5"/>
       <c r="C222" s="5"/>
       <c r="D222" s="5"/>
@@ -5749,7 +5830,7 @@
       <c r="V222" s="5"/>
       <c r="W222" s="7"/>
     </row>
-    <row r="223" spans="2:23">
+    <row r="223" spans="1:23">
       <c r="B223" s="5"/>
       <c r="C223" s="5"/>
       <c r="D223" s="5"/>
@@ -5771,7 +5852,7 @@
       <c r="V223" s="5"/>
       <c r="W223" s="7"/>
     </row>
-    <row r="224" spans="2:23">
+    <row r="224" spans="1:23">
       <c r="B224" s="5"/>
       <c r="C224" s="5"/>
       <c r="D224" s="5"/>
@@ -5882,7 +5963,6 @@
       <c r="W228" s="7"/>
     </row>
     <row r="229" spans="1:23">
-      <c r="A229" s="8"/>
       <c r="B229" s="5"/>
       <c r="C229" s="5"/>
       <c r="D229" s="5"/>
@@ -5927,7 +6007,6 @@
       <c r="W230" s="7"/>
     </row>
     <row r="231" spans="1:23">
-      <c r="A231" s="8"/>
       <c r="B231" s="5"/>
       <c r="C231" s="5"/>
       <c r="D231" s="5"/>
@@ -5950,7 +6029,6 @@
       <c r="W231" s="7"/>
     </row>
     <row r="232" spans="1:23">
-      <c r="A232" s="3"/>
       <c r="B232" s="5"/>
       <c r="C232" s="5"/>
       <c r="D232" s="5"/>
@@ -6013,7 +6091,7 @@
       <c r="S234" s="5"/>
       <c r="T234" s="5"/>
       <c r="U234" s="5"/>
-      <c r="V234" s="1"/>
+      <c r="V234" s="5"/>
       <c r="W234" s="7"/>
     </row>
     <row r="235" spans="1:23">
@@ -6035,11 +6113,10 @@
       <c r="S235" s="5"/>
       <c r="T235" s="5"/>
       <c r="U235" s="5"/>
-      <c r="V235" s="1"/>
+      <c r="V235" s="5"/>
       <c r="W235" s="7"/>
     </row>
     <row r="236" spans="1:23">
-      <c r="A236" s="8"/>
       <c r="B236" s="5"/>
       <c r="C236" s="5"/>
       <c r="D236" s="5"/>
@@ -6103,7 +6180,7 @@
       <c r="S238" s="5"/>
       <c r="T238" s="5"/>
       <c r="U238" s="5"/>
-      <c r="V238" s="1"/>
+      <c r="V238" s="5"/>
       <c r="W238" s="7"/>
     </row>
     <row r="239" spans="1:23">
@@ -6129,6 +6206,7 @@
       <c r="W239" s="7"/>
     </row>
     <row r="240" spans="1:23">
+      <c r="A240" s="8"/>
       <c r="B240" s="5"/>
       <c r="C240" s="5"/>
       <c r="D240" s="5"/>
@@ -6150,7 +6228,8 @@
       <c r="V240" s="5"/>
       <c r="W240" s="7"/>
     </row>
-    <row r="241" spans="2:23">
+    <row r="241" spans="1:23">
+      <c r="A241" s="3"/>
       <c r="B241" s="5"/>
       <c r="C241" s="5"/>
       <c r="D241" s="5"/>
@@ -6169,10 +6248,10 @@
       <c r="S241" s="5"/>
       <c r="T241" s="5"/>
       <c r="U241" s="5"/>
-      <c r="V241" s="1"/>
+      <c r="V241" s="5"/>
       <c r="W241" s="7"/>
     </row>
-    <row r="242" spans="2:23">
+    <row r="242" spans="1:23">
       <c r="B242" s="5"/>
       <c r="C242" s="5"/>
       <c r="D242" s="5"/>
@@ -6191,10 +6270,10 @@
       <c r="S242" s="5"/>
       <c r="T242" s="5"/>
       <c r="U242" s="5"/>
-      <c r="V242" s="1"/>
+      <c r="V242" s="5"/>
       <c r="W242" s="7"/>
     </row>
-    <row r="243" spans="2:23">
+    <row r="243" spans="1:23">
       <c r="B243" s="5"/>
       <c r="C243" s="5"/>
       <c r="D243" s="5"/>
@@ -6216,7 +6295,7 @@
       <c r="V243" s="1"/>
       <c r="W243" s="7"/>
     </row>
-    <row r="244" spans="2:23">
+    <row r="244" spans="1:23">
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
       <c r="D244" s="5"/>
@@ -6238,7 +6317,8 @@
       <c r="V244" s="1"/>
       <c r="W244" s="7"/>
     </row>
-    <row r="245" spans="2:23">
+    <row r="245" spans="1:23">
+      <c r="A245" s="8"/>
       <c r="B245" s="5"/>
       <c r="C245" s="5"/>
       <c r="D245" s="5"/>
@@ -6260,7 +6340,7 @@
       <c r="V245" s="5"/>
       <c r="W245" s="7"/>
     </row>
-    <row r="246" spans="2:23">
+    <row r="246" spans="1:23">
       <c r="B246" s="5"/>
       <c r="C246" s="5"/>
       <c r="D246" s="5"/>
@@ -6282,7 +6362,8 @@
       <c r="V246" s="5"/>
       <c r="W246" s="7"/>
     </row>
-    <row r="247" spans="2:23">
+    <row r="247" spans="1:23">
+      <c r="A247" s="8"/>
       <c r="B247" s="5"/>
       <c r="C247" s="5"/>
       <c r="D247" s="5"/>
@@ -6301,10 +6382,10 @@
       <c r="S247" s="5"/>
       <c r="T247" s="5"/>
       <c r="U247" s="5"/>
-      <c r="V247" s="5"/>
+      <c r="V247" s="1"/>
       <c r="W247" s="7"/>
     </row>
-    <row r="248" spans="2:23">
+    <row r="248" spans="1:23">
       <c r="B248" s="5"/>
       <c r="C248" s="5"/>
       <c r="D248" s="5"/>
@@ -6326,7 +6407,7 @@
       <c r="V248" s="5"/>
       <c r="W248" s="7"/>
     </row>
-    <row r="249" spans="2:23">
+    <row r="249" spans="1:23">
       <c r="B249" s="5"/>
       <c r="C249" s="5"/>
       <c r="D249" s="5"/>
@@ -6345,10 +6426,10 @@
       <c r="S249" s="5"/>
       <c r="T249" s="5"/>
       <c r="U249" s="5"/>
-      <c r="V249" s="1"/>
+      <c r="V249" s="5"/>
       <c r="W249" s="7"/>
     </row>
-    <row r="250" spans="2:23">
+    <row r="250" spans="1:23">
       <c r="B250" s="5"/>
       <c r="C250" s="5"/>
       <c r="D250" s="5"/>
@@ -6370,7 +6451,7 @@
       <c r="V250" s="1"/>
       <c r="W250" s="7"/>
     </row>
-    <row r="251" spans="2:23">
+    <row r="251" spans="1:23">
       <c r="B251" s="5"/>
       <c r="C251" s="5"/>
       <c r="D251" s="5"/>
@@ -6389,10 +6470,10 @@
       <c r="S251" s="5"/>
       <c r="T251" s="5"/>
       <c r="U251" s="5"/>
-      <c r="V251" s="5"/>
+      <c r="V251" s="1"/>
       <c r="W251" s="7"/>
     </row>
-    <row r="252" spans="2:23">
+    <row r="252" spans="1:23">
       <c r="B252" s="5"/>
       <c r="C252" s="5"/>
       <c r="D252" s="5"/>
@@ -6411,10 +6492,10 @@
       <c r="S252" s="5"/>
       <c r="T252" s="5"/>
       <c r="U252" s="5"/>
-      <c r="V252" s="5"/>
+      <c r="V252" s="1"/>
       <c r="W252" s="7"/>
     </row>
-    <row r="253" spans="2:23">
+    <row r="253" spans="1:23">
       <c r="B253" s="5"/>
       <c r="C253" s="5"/>
       <c r="D253" s="5"/>
@@ -6433,10 +6514,10 @@
       <c r="S253" s="5"/>
       <c r="T253" s="5"/>
       <c r="U253" s="5"/>
-      <c r="V253" s="5"/>
+      <c r="V253" s="1"/>
       <c r="W253" s="7"/>
     </row>
-    <row r="254" spans="2:23">
+    <row r="254" spans="1:23">
       <c r="B254" s="5"/>
       <c r="C254" s="5"/>
       <c r="D254" s="5"/>
@@ -6458,7 +6539,7 @@
       <c r="V254" s="5"/>
       <c r="W254" s="7"/>
     </row>
-    <row r="255" spans="2:23">
+    <row r="255" spans="1:23">
       <c r="B255" s="5"/>
       <c r="C255" s="5"/>
       <c r="D255" s="5"/>
@@ -6480,7 +6561,7 @@
       <c r="V255" s="5"/>
       <c r="W255" s="7"/>
     </row>
-    <row r="256" spans="2:23">
+    <row r="256" spans="1:23">
       <c r="B256" s="5"/>
       <c r="C256" s="5"/>
       <c r="D256" s="5"/>
@@ -6543,7 +6624,7 @@
       <c r="S258" s="5"/>
       <c r="T258" s="5"/>
       <c r="U258" s="5"/>
-      <c r="V258" s="5"/>
+      <c r="V258" s="1"/>
       <c r="W258" s="7"/>
     </row>
     <row r="259" spans="2:23">
@@ -6565,7 +6646,7 @@
       <c r="S259" s="5"/>
       <c r="T259" s="5"/>
       <c r="U259" s="5"/>
-      <c r="V259" s="5"/>
+      <c r="V259" s="1"/>
       <c r="W259" s="7"/>
     </row>
     <row r="260" spans="2:23">
@@ -6961,7 +7042,7 @@
       <c r="S277" s="5"/>
       <c r="T277" s="5"/>
       <c r="U277" s="5"/>
-      <c r="V277" s="1"/>
+      <c r="V277" s="5"/>
       <c r="W277" s="7"/>
     </row>
     <row r="278" spans="2:23">
@@ -6983,7 +7064,7 @@
       <c r="S278" s="5"/>
       <c r="T278" s="5"/>
       <c r="U278" s="5"/>
-      <c r="V278" s="1"/>
+      <c r="V278" s="5"/>
       <c r="W278" s="7"/>
     </row>
     <row r="279" spans="2:23">
@@ -7049,7 +7130,7 @@
       <c r="S281" s="5"/>
       <c r="T281" s="5"/>
       <c r="U281" s="5"/>
-      <c r="V281" s="1"/>
+      <c r="V281" s="5"/>
       <c r="W281" s="7"/>
     </row>
     <row r="282" spans="2:23">
@@ -7159,7 +7240,7 @@
       <c r="S286" s="5"/>
       <c r="T286" s="5"/>
       <c r="U286" s="5"/>
-      <c r="V286" s="5"/>
+      <c r="V286" s="1"/>
       <c r="W286" s="7"/>
     </row>
     <row r="287" spans="2:23">
@@ -7181,7 +7262,7 @@
       <c r="S287" s="5"/>
       <c r="T287" s="5"/>
       <c r="U287" s="5"/>
-      <c r="V287" s="5"/>
+      <c r="V287" s="1"/>
       <c r="W287" s="7"/>
     </row>
     <row r="288" spans="2:23">
@@ -7247,7 +7328,7 @@
       <c r="S290" s="5"/>
       <c r="T290" s="5"/>
       <c r="U290" s="5"/>
-      <c r="V290" s="5"/>
+      <c r="V290" s="1"/>
       <c r="W290" s="7"/>
     </row>
     <row r="291" spans="2:23">
@@ -7621,7 +7702,7 @@
       <c r="S307" s="5"/>
       <c r="T307" s="5"/>
       <c r="U307" s="5"/>
-      <c r="V307" s="1"/>
+      <c r="V307" s="5"/>
       <c r="W307" s="7"/>
     </row>
     <row r="308" spans="2:23">
@@ -7643,7 +7724,7 @@
       <c r="S308" s="5"/>
       <c r="T308" s="5"/>
       <c r="U308" s="5"/>
-      <c r="V308" s="1"/>
+      <c r="V308" s="5"/>
       <c r="W308" s="7"/>
     </row>
     <row r="309" spans="2:23">
@@ -7665,7 +7746,7 @@
       <c r="S309" s="5"/>
       <c r="T309" s="5"/>
       <c r="U309" s="5"/>
-      <c r="V309" s="1"/>
+      <c r="V309" s="5"/>
       <c r="W309" s="7"/>
     </row>
     <row r="310" spans="2:23">
@@ -7687,7 +7768,7 @@
       <c r="S310" s="5"/>
       <c r="T310" s="5"/>
       <c r="U310" s="5"/>
-      <c r="V310" s="1"/>
+      <c r="V310" s="5"/>
       <c r="W310" s="7"/>
     </row>
     <row r="311" spans="2:23">
@@ -7709,7 +7790,7 @@
       <c r="S311" s="5"/>
       <c r="T311" s="5"/>
       <c r="U311" s="5"/>
-      <c r="V311" s="1"/>
+      <c r="V311" s="5"/>
       <c r="W311" s="7"/>
     </row>
     <row r="312" spans="2:23">
@@ -7863,7 +7944,7 @@
       <c r="S318" s="5"/>
       <c r="T318" s="5"/>
       <c r="U318" s="5"/>
-      <c r="V318" s="5"/>
+      <c r="V318" s="1"/>
       <c r="W318" s="7"/>
     </row>
     <row r="319" spans="2:23">
@@ -7885,7 +7966,7 @@
       <c r="S319" s="5"/>
       <c r="T319" s="5"/>
       <c r="U319" s="5"/>
-      <c r="V319" s="5"/>
+      <c r="V319" s="1"/>
       <c r="W319" s="7"/>
     </row>
     <row r="320" spans="2:23">
@@ -7929,7 +8010,7 @@
       <c r="S321" s="5"/>
       <c r="T321" s="5"/>
       <c r="U321" s="5"/>
-      <c r="V321" s="1"/>
+      <c r="V321" s="5"/>
       <c r="W321" s="7"/>
     </row>
     <row r="322" spans="2:23">
@@ -8017,7 +8098,7 @@
       <c r="S325" s="5"/>
       <c r="T325" s="5"/>
       <c r="U325" s="5"/>
-      <c r="V325" s="5"/>
+      <c r="V325" s="1"/>
       <c r="W325" s="7"/>
     </row>
     <row r="326" spans="2:23">
@@ -8039,7 +8120,7 @@
       <c r="S326" s="5"/>
       <c r="T326" s="5"/>
       <c r="U326" s="5"/>
-      <c r="V326" s="5"/>
+      <c r="V326" s="1"/>
       <c r="W326" s="7"/>
     </row>
     <row r="327" spans="2:23">
@@ -8105,7 +8186,7 @@
       <c r="S329" s="5"/>
       <c r="T329" s="5"/>
       <c r="U329" s="5"/>
-      <c r="V329" s="5"/>
+      <c r="V329" s="1"/>
       <c r="W329" s="7"/>
     </row>
     <row r="330" spans="2:23">
@@ -8127,7 +8208,7 @@
       <c r="S330" s="5"/>
       <c r="T330" s="5"/>
       <c r="U330" s="5"/>
-      <c r="V330" s="5"/>
+      <c r="V330" s="1"/>
       <c r="W330" s="7"/>
     </row>
     <row r="331" spans="2:23">
@@ -8303,7 +8384,7 @@
       <c r="S338" s="5"/>
       <c r="T338" s="5"/>
       <c r="U338" s="5"/>
-      <c r="V338" s="1"/>
+      <c r="V338" s="5"/>
       <c r="W338" s="7"/>
     </row>
     <row r="339" spans="2:23">
@@ -8325,7 +8406,7 @@
       <c r="S339" s="5"/>
       <c r="T339" s="5"/>
       <c r="U339" s="5"/>
-      <c r="V339" s="1"/>
+      <c r="V339" s="5"/>
       <c r="W339" s="7"/>
     </row>
     <row r="340" spans="2:23">
@@ -8479,7 +8560,7 @@
       <c r="S346" s="5"/>
       <c r="T346" s="5"/>
       <c r="U346" s="5"/>
-      <c r="V346" s="1"/>
+      <c r="V346" s="5"/>
       <c r="W346" s="7"/>
     </row>
     <row r="347" spans="2:23">
@@ -8523,7 +8604,7 @@
       <c r="S348" s="5"/>
       <c r="T348" s="5"/>
       <c r="U348" s="5"/>
-      <c r="V348" s="5"/>
+      <c r="V348" s="1"/>
       <c r="W348" s="7"/>
     </row>
     <row r="349" spans="2:23">
@@ -8567,7 +8648,7 @@
       <c r="S350" s="5"/>
       <c r="T350" s="5"/>
       <c r="U350" s="5"/>
-      <c r="V350" s="1"/>
+      <c r="V350" s="5"/>
       <c r="W350" s="7"/>
     </row>
     <row r="351" spans="2:23">
@@ -8677,7 +8758,7 @@
       <c r="S355" s="5"/>
       <c r="T355" s="5"/>
       <c r="U355" s="5"/>
-      <c r="V355" s="5"/>
+      <c r="V355" s="1"/>
       <c r="W355" s="7"/>
     </row>
     <row r="356" spans="2:23">
@@ -8699,7 +8780,7 @@
       <c r="S356" s="5"/>
       <c r="T356" s="5"/>
       <c r="U356" s="5"/>
-      <c r="V356" s="5"/>
+      <c r="V356" s="1"/>
       <c r="W356" s="7"/>
     </row>
     <row r="357" spans="2:23">
@@ -8765,7 +8846,7 @@
       <c r="S359" s="5"/>
       <c r="T359" s="5"/>
       <c r="U359" s="5"/>
-      <c r="V359" s="5"/>
+      <c r="V359" s="1"/>
       <c r="W359" s="7"/>
     </row>
     <row r="360" spans="2:23">
@@ -9051,7 +9132,7 @@
       <c r="S372" s="5"/>
       <c r="T372" s="5"/>
       <c r="U372" s="5"/>
-      <c r="V372" s="1"/>
+      <c r="V372" s="5"/>
       <c r="W372" s="7"/>
     </row>
     <row r="373" spans="2:23">
@@ -9073,7 +9154,7 @@
       <c r="S373" s="5"/>
       <c r="T373" s="5"/>
       <c r="U373" s="5"/>
-      <c r="V373" s="1"/>
+      <c r="V373" s="5"/>
       <c r="W373" s="7"/>
     </row>
     <row r="374" spans="2:23">
@@ -9095,7 +9176,7 @@
       <c r="S374" s="5"/>
       <c r="T374" s="5"/>
       <c r="U374" s="5"/>
-      <c r="V374" s="1"/>
+      <c r="V374" s="5"/>
       <c r="W374" s="7"/>
     </row>
     <row r="375" spans="2:23">
@@ -9117,7 +9198,7 @@
       <c r="S375" s="5"/>
       <c r="T375" s="5"/>
       <c r="U375" s="5"/>
-      <c r="V375" s="1"/>
+      <c r="V375" s="5"/>
       <c r="W375" s="7"/>
     </row>
     <row r="376" spans="2:23">
@@ -9139,7 +9220,7 @@
       <c r="S376" s="5"/>
       <c r="T376" s="5"/>
       <c r="U376" s="5"/>
-      <c r="V376" s="1"/>
+      <c r="V376" s="5"/>
       <c r="W376" s="7"/>
     </row>
     <row r="377" spans="2:23">
@@ -9293,7 +9374,7 @@
       <c r="S383" s="5"/>
       <c r="T383" s="5"/>
       <c r="U383" s="5"/>
-      <c r="V383" s="5"/>
+      <c r="V383" s="1"/>
       <c r="W383" s="7"/>
     </row>
     <row r="384" spans="2:23">
@@ -9315,10 +9396,10 @@
       <c r="S384" s="5"/>
       <c r="T384" s="5"/>
       <c r="U384" s="5"/>
-      <c r="V384" s="5"/>
+      <c r="V384" s="1"/>
       <c r="W384" s="7"/>
     </row>
-    <row r="385" spans="1:23">
+    <row r="385" spans="2:23">
       <c r="B385" s="5"/>
       <c r="C385" s="5"/>
       <c r="D385" s="5"/>
@@ -9340,7 +9421,7 @@
       <c r="V385" s="1"/>
       <c r="W385" s="7"/>
     </row>
-    <row r="386" spans="1:23">
+    <row r="386" spans="2:23">
       <c r="B386" s="5"/>
       <c r="C386" s="5"/>
       <c r="D386" s="5"/>
@@ -9359,10 +9440,10 @@
       <c r="S386" s="5"/>
       <c r="T386" s="5"/>
       <c r="U386" s="5"/>
-      <c r="V386" s="1"/>
+      <c r="V386" s="5"/>
       <c r="W386" s="7"/>
     </row>
-    <row r="387" spans="1:23">
+    <row r="387" spans="2:23">
       <c r="B387" s="5"/>
       <c r="C387" s="5"/>
       <c r="D387" s="5"/>
@@ -9384,7 +9465,7 @@
       <c r="V387" s="5"/>
       <c r="W387" s="7"/>
     </row>
-    <row r="388" spans="1:23">
+    <row r="388" spans="2:23">
       <c r="B388" s="5"/>
       <c r="C388" s="5"/>
       <c r="D388" s="5"/>
@@ -9406,7 +9487,7 @@
       <c r="V388" s="5"/>
       <c r="W388" s="7"/>
     </row>
-    <row r="389" spans="1:23">
+    <row r="389" spans="2:23">
       <c r="B389" s="5"/>
       <c r="C389" s="5"/>
       <c r="D389" s="5"/>
@@ -9428,7 +9509,7 @@
       <c r="V389" s="5"/>
       <c r="W389" s="7"/>
     </row>
-    <row r="390" spans="1:23">
+    <row r="390" spans="2:23">
       <c r="B390" s="5"/>
       <c r="C390" s="5"/>
       <c r="D390" s="5"/>
@@ -9447,10 +9528,10 @@
       <c r="S390" s="5"/>
       <c r="T390" s="5"/>
       <c r="U390" s="5"/>
-      <c r="V390" s="5"/>
+      <c r="V390" s="1"/>
       <c r="W390" s="7"/>
     </row>
-    <row r="391" spans="1:23">
+    <row r="391" spans="2:23">
       <c r="B391" s="5"/>
       <c r="C391" s="5"/>
       <c r="D391" s="5"/>
@@ -9469,10 +9550,10 @@
       <c r="S391" s="5"/>
       <c r="T391" s="5"/>
       <c r="U391" s="5"/>
-      <c r="V391" s="5"/>
+      <c r="V391" s="1"/>
       <c r="W391" s="7"/>
     </row>
-    <row r="392" spans="1:23">
+    <row r="392" spans="2:23">
       <c r="B392" s="5"/>
       <c r="C392" s="5"/>
       <c r="D392" s="5"/>
@@ -9494,7 +9575,7 @@
       <c r="V392" s="5"/>
       <c r="W392" s="7"/>
     </row>
-    <row r="393" spans="1:23">
+    <row r="393" spans="2:23">
       <c r="B393" s="5"/>
       <c r="C393" s="5"/>
       <c r="D393" s="5"/>
@@ -9516,7 +9597,7 @@
       <c r="V393" s="5"/>
       <c r="W393" s="7"/>
     </row>
-    <row r="394" spans="1:23">
+    <row r="394" spans="2:23">
       <c r="B394" s="5"/>
       <c r="C394" s="5"/>
       <c r="D394" s="5"/>
@@ -9535,10 +9616,10 @@
       <c r="S394" s="5"/>
       <c r="T394" s="5"/>
       <c r="U394" s="5"/>
-      <c r="V394" s="5"/>
+      <c r="V394" s="1"/>
       <c r="W394" s="7"/>
     </row>
-    <row r="395" spans="1:23">
+    <row r="395" spans="2:23">
       <c r="B395" s="5"/>
       <c r="C395" s="5"/>
       <c r="D395" s="5"/>
@@ -9557,10 +9638,10 @@
       <c r="S395" s="5"/>
       <c r="T395" s="5"/>
       <c r="U395" s="5"/>
-      <c r="V395" s="5"/>
+      <c r="V395" s="1"/>
       <c r="W395" s="7"/>
     </row>
-    <row r="396" spans="1:23">
+    <row r="396" spans="2:23">
       <c r="B396" s="5"/>
       <c r="C396" s="5"/>
       <c r="D396" s="5"/>
@@ -9582,7 +9663,7 @@
       <c r="V396" s="5"/>
       <c r="W396" s="7"/>
     </row>
-    <row r="397" spans="1:23">
+    <row r="397" spans="2:23">
       <c r="B397" s="5"/>
       <c r="C397" s="5"/>
       <c r="D397" s="5"/>
@@ -9604,7 +9685,7 @@
       <c r="V397" s="5"/>
       <c r="W397" s="7"/>
     </row>
-    <row r="398" spans="1:23">
+    <row r="398" spans="2:23">
       <c r="B398" s="5"/>
       <c r="C398" s="5"/>
       <c r="D398" s="5"/>
@@ -9626,7 +9707,7 @@
       <c r="V398" s="5"/>
       <c r="W398" s="7"/>
     </row>
-    <row r="399" spans="1:23">
+    <row r="399" spans="2:23">
       <c r="B399" s="5"/>
       <c r="C399" s="5"/>
       <c r="D399" s="5"/>
@@ -9648,8 +9729,7 @@
       <c r="V399" s="5"/>
       <c r="W399" s="7"/>
     </row>
-    <row r="400" spans="1:23">
-      <c r="A400" s="8"/>
+    <row r="400" spans="2:23">
       <c r="B400" s="5"/>
       <c r="C400" s="5"/>
       <c r="D400" s="5"/>
@@ -9734,7 +9814,7 @@
       <c r="S403" s="5"/>
       <c r="T403" s="5"/>
       <c r="U403" s="5"/>
-      <c r="V403" s="1"/>
+      <c r="V403" s="5"/>
       <c r="W403" s="7"/>
     </row>
     <row r="404" spans="1:23">
@@ -9756,7 +9836,7 @@
       <c r="S404" s="5"/>
       <c r="T404" s="5"/>
       <c r="U404" s="5"/>
-      <c r="V404" s="1"/>
+      <c r="V404" s="5"/>
       <c r="W404" s="7"/>
     </row>
     <row r="405" spans="1:23">
@@ -9804,7 +9884,6 @@
       <c r="W406" s="7"/>
     </row>
     <row r="407" spans="1:23">
-      <c r="A407" s="3"/>
       <c r="B407" s="5"/>
       <c r="C407" s="5"/>
       <c r="D407" s="5"/>
@@ -9827,7 +9906,6 @@
       <c r="W407" s="7"/>
     </row>
     <row r="408" spans="1:23">
-      <c r="A408" s="8"/>
       <c r="B408" s="5"/>
       <c r="C408" s="5"/>
       <c r="D408" s="5"/>
@@ -9850,6 +9928,7 @@
       <c r="W408" s="7"/>
     </row>
     <row r="409" spans="1:23">
+      <c r="A409" s="8"/>
       <c r="B409" s="5"/>
       <c r="C409" s="5"/>
       <c r="D409" s="5"/>
@@ -9912,7 +9991,7 @@
       <c r="S411" s="5"/>
       <c r="T411" s="5"/>
       <c r="U411" s="5"/>
-      <c r="V411" s="1"/>
+      <c r="V411" s="5"/>
       <c r="W411" s="7"/>
     </row>
     <row r="412" spans="1:23">
@@ -9956,7 +10035,7 @@
       <c r="S413" s="5"/>
       <c r="T413" s="5"/>
       <c r="U413" s="5"/>
-      <c r="V413" s="5"/>
+      <c r="V413" s="1"/>
       <c r="W413" s="7"/>
     </row>
     <row r="414" spans="1:23">
@@ -10000,8 +10079,208 @@
       <c r="S415" s="5"/>
       <c r="T415" s="5"/>
       <c r="U415" s="5"/>
-      <c r="V415" s="1"/>
+      <c r="V415" s="5"/>
       <c r="W415" s="7"/>
+    </row>
+    <row r="416" spans="1:23">
+      <c r="A416" s="3"/>
+      <c r="B416" s="5"/>
+      <c r="C416" s="5"/>
+      <c r="D416" s="5"/>
+      <c r="E416" s="5"/>
+      <c r="H416" s="5"/>
+      <c r="I416" s="5"/>
+      <c r="J416" s="5"/>
+      <c r="K416" s="5"/>
+      <c r="L416" s="5"/>
+      <c r="M416" s="6"/>
+      <c r="N416" s="5"/>
+      <c r="O416" s="5"/>
+      <c r="P416" s="5"/>
+      <c r="Q416" s="5"/>
+      <c r="R416" s="5"/>
+      <c r="S416" s="5"/>
+      <c r="T416" s="5"/>
+      <c r="U416" s="5"/>
+      <c r="V416" s="5"/>
+      <c r="W416" s="7"/>
+    </row>
+    <row r="417" spans="1:23">
+      <c r="A417" s="8"/>
+      <c r="B417" s="5"/>
+      <c r="C417" s="5"/>
+      <c r="D417" s="5"/>
+      <c r="E417" s="5"/>
+      <c r="H417" s="5"/>
+      <c r="I417" s="5"/>
+      <c r="J417" s="5"/>
+      <c r="K417" s="5"/>
+      <c r="L417" s="5"/>
+      <c r="M417" s="6"/>
+      <c r="N417" s="5"/>
+      <c r="O417" s="5"/>
+      <c r="P417" s="5"/>
+      <c r="Q417" s="5"/>
+      <c r="R417" s="5"/>
+      <c r="S417" s="5"/>
+      <c r="T417" s="5"/>
+      <c r="U417" s="5"/>
+      <c r="V417" s="5"/>
+      <c r="W417" s="7"/>
+    </row>
+    <row r="418" spans="1:23">
+      <c r="B418" s="5"/>
+      <c r="C418" s="5"/>
+      <c r="D418" s="5"/>
+      <c r="E418" s="5"/>
+      <c r="H418" s="5"/>
+      <c r="I418" s="5"/>
+      <c r="J418" s="5"/>
+      <c r="K418" s="5"/>
+      <c r="L418" s="5"/>
+      <c r="M418" s="6"/>
+      <c r="N418" s="5"/>
+      <c r="O418" s="5"/>
+      <c r="P418" s="5"/>
+      <c r="Q418" s="5"/>
+      <c r="R418" s="5"/>
+      <c r="S418" s="5"/>
+      <c r="T418" s="5"/>
+      <c r="U418" s="5"/>
+      <c r="V418" s="5"/>
+      <c r="W418" s="7"/>
+    </row>
+    <row r="419" spans="1:23">
+      <c r="B419" s="5"/>
+      <c r="C419" s="5"/>
+      <c r="D419" s="5"/>
+      <c r="E419" s="5"/>
+      <c r="H419" s="5"/>
+      <c r="I419" s="5"/>
+      <c r="J419" s="5"/>
+      <c r="K419" s="5"/>
+      <c r="L419" s="5"/>
+      <c r="M419" s="6"/>
+      <c r="N419" s="5"/>
+      <c r="O419" s="5"/>
+      <c r="P419" s="5"/>
+      <c r="Q419" s="5"/>
+      <c r="R419" s="5"/>
+      <c r="S419" s="5"/>
+      <c r="T419" s="5"/>
+      <c r="U419" s="5"/>
+      <c r="V419" s="5"/>
+      <c r="W419" s="7"/>
+    </row>
+    <row r="420" spans="1:23">
+      <c r="B420" s="5"/>
+      <c r="C420" s="5"/>
+      <c r="D420" s="5"/>
+      <c r="E420" s="5"/>
+      <c r="H420" s="5"/>
+      <c r="I420" s="5"/>
+      <c r="J420" s="5"/>
+      <c r="K420" s="5"/>
+      <c r="L420" s="5"/>
+      <c r="M420" s="6"/>
+      <c r="N420" s="5"/>
+      <c r="O420" s="5"/>
+      <c r="P420" s="5"/>
+      <c r="Q420" s="5"/>
+      <c r="R420" s="5"/>
+      <c r="S420" s="5"/>
+      <c r="T420" s="5"/>
+      <c r="U420" s="5"/>
+      <c r="V420" s="1"/>
+      <c r="W420" s="7"/>
+    </row>
+    <row r="421" spans="1:23">
+      <c r="B421" s="5"/>
+      <c r="C421" s="5"/>
+      <c r="D421" s="5"/>
+      <c r="E421" s="5"/>
+      <c r="H421" s="5"/>
+      <c r="I421" s="5"/>
+      <c r="J421" s="5"/>
+      <c r="K421" s="5"/>
+      <c r="L421" s="5"/>
+      <c r="M421" s="6"/>
+      <c r="N421" s="5"/>
+      <c r="O421" s="5"/>
+      <c r="P421" s="5"/>
+      <c r="Q421" s="5"/>
+      <c r="R421" s="5"/>
+      <c r="S421" s="5"/>
+      <c r="T421" s="5"/>
+      <c r="U421" s="5"/>
+      <c r="V421" s="1"/>
+      <c r="W421" s="7"/>
+    </row>
+    <row r="422" spans="1:23">
+      <c r="B422" s="5"/>
+      <c r="C422" s="5"/>
+      <c r="D422" s="5"/>
+      <c r="E422" s="5"/>
+      <c r="H422" s="5"/>
+      <c r="I422" s="5"/>
+      <c r="J422" s="5"/>
+      <c r="K422" s="5"/>
+      <c r="L422" s="5"/>
+      <c r="M422" s="6"/>
+      <c r="N422" s="5"/>
+      <c r="O422" s="5"/>
+      <c r="P422" s="5"/>
+      <c r="Q422" s="5"/>
+      <c r="R422" s="5"/>
+      <c r="S422" s="5"/>
+      <c r="T422" s="5"/>
+      <c r="U422" s="5"/>
+      <c r="V422" s="5"/>
+      <c r="W422" s="7"/>
+    </row>
+    <row r="423" spans="1:23">
+      <c r="B423" s="5"/>
+      <c r="C423" s="5"/>
+      <c r="D423" s="5"/>
+      <c r="E423" s="5"/>
+      <c r="H423" s="5"/>
+      <c r="I423" s="5"/>
+      <c r="J423" s="5"/>
+      <c r="K423" s="5"/>
+      <c r="L423" s="5"/>
+      <c r="M423" s="6"/>
+      <c r="N423" s="5"/>
+      <c r="O423" s="5"/>
+      <c r="P423" s="5"/>
+      <c r="Q423" s="5"/>
+      <c r="R423" s="5"/>
+      <c r="S423" s="5"/>
+      <c r="T423" s="5"/>
+      <c r="U423" s="5"/>
+      <c r="V423" s="5"/>
+      <c r="W423" s="7"/>
+    </row>
+    <row r="424" spans="1:23">
+      <c r="B424" s="5"/>
+      <c r="C424" s="5"/>
+      <c r="D424" s="5"/>
+      <c r="E424" s="5"/>
+      <c r="H424" s="5"/>
+      <c r="I424" s="5"/>
+      <c r="J424" s="5"/>
+      <c r="K424" s="5"/>
+      <c r="L424" s="5"/>
+      <c r="M424" s="6"/>
+      <c r="N424" s="5"/>
+      <c r="O424" s="5"/>
+      <c r="P424" s="5"/>
+      <c r="Q424" s="5"/>
+      <c r="R424" s="5"/>
+      <c r="S424" s="5"/>
+      <c r="T424" s="5"/>
+      <c r="U424" s="5"/>
+      <c r="V424" s="1"/>
+      <c r="W424" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>